<commit_message>
Clebina não upou :c
clebina não upou :c
</commit_message>
<xml_diff>
--- a/Fichas/Tormenta/Ficha Cleber.xlsx
+++ b/Fichas/Tormenta/Ficha Cleber.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashzi\OneDrive\Documentos\GitHub\RPG\Fichas\Tormenta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D672967-C19A-423F-82C9-9A300DB2C82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2EEBB4-A154-4867-A32A-0786FBC49EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{B06712FB-01E1-4038-87FF-6E8B7BD1F9D8}"/>
   </bookViews>
@@ -2470,7 +2470,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2479,7 +2479,7 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2535,230 +2535,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="42">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF231F20"/>
-        <name val="Palatino Linotype"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF231F20"/>
-        <name val="Palatino Linotype"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF231F20"/>
-        <name val="Palatino Linotype"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color rgb="FF231F20"/>
-        <name val="Palatino Linotype"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thick">
-          <color indexed="64"/>
-        </left>
-        <right style="thick">
-          <color indexed="64"/>
-        </right>
-        <top style="thick">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thick">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF231F20"/>
-        <name val="Palatino Linotype"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFD7CFCB"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4021,6 +3797,230 @@
         </horizontal>
       </border>
     </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF231F20"/>
+        <name val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF231F20"/>
+        <name val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF231F20"/>
+        <name val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color rgb="FF231F20"/>
+        <name val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thick">
+          <color indexed="64"/>
+        </left>
+        <right style="thick">
+          <color indexed="64"/>
+        </right>
+        <top style="thick">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thick">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF231F20"/>
+        <name val="Palatino Linotype"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFD7CFCB"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4035,13 +4035,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{341B94BB-993F-46E0-8D20-25D8B8DFC9D2}" name="Tabela2" displayName="Tabela2" ref="B2:E35" totalsRowShown="0" headerRowDxfId="7" headerRowBorderDxfId="5" tableBorderDxfId="6" totalsRowBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{341B94BB-993F-46E0-8D20-25D8B8DFC9D2}" name="Tabela2" displayName="Tabela2" ref="B2:E35" totalsRowShown="0" headerRowDxfId="41" headerRowBorderDxfId="40" tableBorderDxfId="39" totalsRowBorderDxfId="38">
   <autoFilter ref="B2:E35" xr:uid="{341B94BB-993F-46E0-8D20-25D8B8DFC9D2}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1894870-874E-4AAD-A247-ECC662F48358}" name="Magia" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{E9C52482-94DF-400D-B27D-3BB0A2CD6FB4}" name="Tipo" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{79E6BF69-750F-4120-9C22-CBF48EC98822}" name="Círculo" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{13264AB4-FFD5-4BB3-BAD2-D832AAF7A08F}" name="Custo" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{D1894870-874E-4AAD-A247-ECC662F48358}" name="Magia" dataDxfId="37"/>
+    <tableColumn id="4" xr3:uid="{E9C52482-94DF-400D-B27D-3BB0A2CD6FB4}" name="Tipo" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{79E6BF69-750F-4120-9C22-CBF48EC98822}" name="Círculo" dataDxfId="35"/>
+    <tableColumn id="3" xr3:uid="{13264AB4-FFD5-4BB3-BAD2-D832AAF7A08F}" name="Custo" dataDxfId="34">
       <calculatedColumnFormula>IFERROR(VLOOKUP(D3,$G$3:$H$7,2,FALSE)^2*10,"")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4050,64 +4050,64 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9B38B72-5BEC-4A97-A0DA-A810BF14F697}" name="Tabela1" displayName="Tabela1" ref="B2:M33" totalsRowShown="0" headerRowDxfId="41" dataDxfId="39" headerRowBorderDxfId="40" tableBorderDxfId="38" totalsRowBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E9B38B72-5BEC-4A97-A0DA-A810BF14F697}" name="Tabela1" displayName="Tabela1" ref="B2:M33" totalsRowShown="0" headerRowDxfId="33" dataDxfId="31" headerRowBorderDxfId="32" tableBorderDxfId="30" totalsRowBorderDxfId="29">
   <autoFilter ref="B2:M33" xr:uid="{E9B38B72-5BEC-4A97-A0DA-A810BF14F697}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M33">
     <sortCondition ref="B2:B33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{35823DB3-F1AE-4CDE-BCEB-3F67A161199D}" name="Perícia" dataDxfId="36"/>
-    <tableColumn id="11" xr3:uid="{71D30AF6-6ECB-4DCC-B970-0C8671D1D99E}" name="ATR" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{F48A0B7A-BF4E-4E96-855A-EF5F80CD02AF}" name="MOD" dataDxfId="34">
+    <tableColumn id="1" xr3:uid="{35823DB3-F1AE-4CDE-BCEB-3F67A161199D}" name="Perícia" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{71D30AF6-6ECB-4DCC-B970-0C8671D1D99E}" name="ATR" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{F48A0B7A-BF4E-4E96-855A-EF5F80CD02AF}" name="MOD" dataDxfId="26">
       <calculatedColumnFormula>VLOOKUP(C3,Cleber!$B$3:$D$8,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{A5C55ADC-017F-4BF3-96EE-DA8B584D4A98}" name="1/2 Nível" dataDxfId="33">
+    <tableColumn id="3" xr3:uid="{A5C55ADC-017F-4BF3-96EE-DA8B584D4A98}" name="1/2 Nível" dataDxfId="25">
       <calculatedColumnFormula>VLOOKUP(Cleber!$G$2,'uns dados aí'!$I$3:$J$22,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{271DCFED-97F3-476E-9BF9-01CA669D22C9}" name="Treino" dataDxfId="32">
+    <tableColumn id="4" xr3:uid="{271DCFED-97F3-476E-9BF9-01CA669D22C9}" name="Treino" dataDxfId="24">
       <calculatedColumnFormula>IF(Tabela1[[#This Row],[Treinada?]]="sim",VLOOKUP(Cleber!$G$2,'uns dados aí'!$E$2:$F$4,2,TRUE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0597BDAA-ECFD-4424-8BC9-0A2726873A2D}" name="Raça" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{DC4DD309-E0D5-4BFA-B599-712B0D96915F}" name="Bônus" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{4B403395-1BD1-4EED-8C7D-DFC601AD6CFC}" name="Bônus Habilidade" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{FA043140-F4F5-450A-8642-B2838683E293}" name="Total" dataDxfId="28">
+    <tableColumn id="10" xr3:uid="{0597BDAA-ECFD-4424-8BC9-0A2726873A2D}" name="Raça" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{DC4DD309-E0D5-4BFA-B599-712B0D96915F}" name="Bônus" dataDxfId="22"/>
+    <tableColumn id="9" xr3:uid="{4B403395-1BD1-4EED-8C7D-DFC601AD6CFC}" name="Bônus Habilidade" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{FA043140-F4F5-450A-8642-B2838683E293}" name="Total" dataDxfId="20">
       <calculatedColumnFormula>SUM(Tabela1[[#This Row],[MOD]:[Bônus Habilidade]])-IF(Tabela1[[#This Row],[Penalidade de Armadura?]]="sim",Cleber!$D$16,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{32CFEA9E-CDB7-467A-9741-E969780B88CF}" name="Treinada?" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{4D510E34-D284-49F1-9685-C49F70168A12}" name="Somente Treinada?" dataDxfId="26"/>
-    <tableColumn id="8" xr3:uid="{DA0D8D90-A3BF-4F51-8AAE-F48C1576B17E}" name="Penalidade de Armadura?" dataDxfId="25"/>
+    <tableColumn id="7" xr3:uid="{32CFEA9E-CDB7-467A-9741-E969780B88CF}" name="Treinada?" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{4D510E34-D284-49F1-9685-C49F70168A12}" name="Somente Treinada?" dataDxfId="18"/>
+    <tableColumn id="8" xr3:uid="{DA0D8D90-A3BF-4F51-8AAE-F48C1576B17E}" name="Penalidade de Armadura?" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{45C4D9DD-A352-4A98-A4EA-69024F44BE5F}" name="Tabela14" displayName="Tabela14" ref="B2:M33" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{45C4D9DD-A352-4A98-A4EA-69024F44BE5F}" name="Tabela14" displayName="Tabela14" ref="B2:M33" totalsRowShown="0" headerRowDxfId="16" dataDxfId="14" headerRowBorderDxfId="15" tableBorderDxfId="13" totalsRowBorderDxfId="12">
   <autoFilter ref="B2:M33" xr:uid="{E9B38B72-5BEC-4A97-A0DA-A810BF14F697}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:M33">
     <sortCondition ref="B2:B33"/>
   </sortState>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{519E1489-C314-4404-A0DD-09AC6888B0FF}" name="Perícia" dataDxfId="19"/>
-    <tableColumn id="11" xr3:uid="{F57CB9B5-4E42-4252-9D3F-1268826FED7D}" name="ATR" dataDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{729B8C64-280C-4BDA-B1DA-7008359BC959}" name="MOD" dataDxfId="17">
+    <tableColumn id="1" xr3:uid="{519E1489-C314-4404-A0DD-09AC6888B0FF}" name="Perícia" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{F57CB9B5-4E42-4252-9D3F-1268826FED7D}" name="ATR" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{729B8C64-280C-4BDA-B1DA-7008359BC959}" name="MOD" dataDxfId="9">
       <calculatedColumnFormula>VLOOKUP(C3,Cleber!$B$3:$D$8,3,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B2896C73-B008-4753-B047-CBF5947F4947}" name="1/2 Nível" dataDxfId="16">
+    <tableColumn id="3" xr3:uid="{B2896C73-B008-4753-B047-CBF5947F4947}" name="1/2 Nível" dataDxfId="8">
       <calculatedColumnFormula>VLOOKUP(Cleber!$G$2,'uns dados aí'!$I$3:$J$22,2,FALSE)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0461CFF1-B44B-490B-9AB9-D95DD1510414}" name="Treino" dataDxfId="15">
+    <tableColumn id="4" xr3:uid="{0461CFF1-B44B-490B-9AB9-D95DD1510414}" name="Treino" dataDxfId="7">
       <calculatedColumnFormula>IF(Tabela14[[#This Row],[Treinada?]]="sim",VLOOKUP(Cleber!$G$2,'uns dados aí'!$E$2:$F$4,2,TRUE),"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9329C84C-824D-4447-A7CA-425033AD5947}" name="Raça" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{9B28FA64-F7B3-4CAF-8C77-540A15A93184}" name="Bônus" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{5C865FA7-8036-4B5F-92C5-F4866E4A2409}" name="Bônus Habilidade" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{B65AFDB5-6A6F-4BE3-ADB2-9497F98B9FC3}" name="Total" dataDxfId="11">
+    <tableColumn id="10" xr3:uid="{9329C84C-824D-4447-A7CA-425033AD5947}" name="Raça" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{9B28FA64-F7B3-4CAF-8C77-540A15A93184}" name="Bônus" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{5C865FA7-8036-4B5F-92C5-F4866E4A2409}" name="Bônus Habilidade" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{B65AFDB5-6A6F-4BE3-ADB2-9497F98B9FC3}" name="Total" dataDxfId="3">
       <calculatedColumnFormula>SUM(Tabela14[[#This Row],[MOD]:[Bônus Habilidade]])-IF(Tabela14[[#This Row],[Penalidade de Armadura?]]="sim",Cleber!D16,0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{79CD8B55-E5C5-4C34-A4BF-7D04F218CCEF}" name="Treinada?" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{59ADF3CE-A6A5-4C36-A35C-28B49FE674B9}" name="Somente Treinada?" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{F4A691E7-DE8B-4B5A-92F4-6623CB4C3A63}" name="Penalidade de Armadura?" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{79CD8B55-E5C5-4C34-A4BF-7D04F218CCEF}" name="Treinada?" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{59ADF3CE-A6A5-4C36-A35C-28B49FE674B9}" name="Somente Treinada?" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{F4A691E7-DE8B-4B5A-92F4-6623CB4C3A63}" name="Penalidade de Armadura?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4666,7 +4666,7 @@
         <v>95</v>
       </c>
       <c r="G10" s="84">
-        <v>3000</v>
+        <v>4600</v>
       </c>
       <c r="H10" s="85"/>
       <c r="K10" s="4">
@@ -4978,7 +4978,7 @@
       <c r="M4" s="63"/>
     </row>
     <row r="5" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="92" t="s">
+      <c r="B5" s="95" t="s">
         <v>35</v>
       </c>
       <c r="C5" s="90"/>
@@ -5018,7 +5018,7 @@
       <c r="M6" s="63"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="95" t="s">
         <v>37</v>
       </c>
       <c r="C7" s="93"/>
@@ -5058,7 +5058,7 @@
       <c r="M8" s="63"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="95" t="s">
         <v>39</v>
       </c>
       <c r="C9" s="93"/>
@@ -5090,7 +5090,7 @@
       <c r="M10" s="63"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="92" t="s">
+      <c r="B11" s="95" t="s">
         <v>41</v>
       </c>
       <c r="C11" s="93"/>
@@ -5122,7 +5122,7 @@
       <c r="M12" s="63"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B13" s="92" t="s">
+      <c r="B13" s="95" t="s">
         <v>85</v>
       </c>
       <c r="C13" s="93"/>
@@ -5151,7 +5151,7 @@
       <c r="M14" s="63"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B15" s="92" t="s">
+      <c r="B15" s="95" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="93"/>
@@ -5175,7 +5175,7 @@
       <c r="M16" s="63"/>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B17" s="92" t="s">
+      <c r="B17" s="95" t="s">
         <v>84</v>
       </c>
       <c r="C17" s="93"/>
@@ -5199,7 +5199,7 @@
       <c r="M18" s="63"/>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="95" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="93"/>
@@ -5223,7 +5223,7 @@
       <c r="M20" s="63"/>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B21" s="92" t="s">
+      <c r="B21" s="95" t="s">
         <v>92</v>
       </c>
       <c r="C21" s="93"/>
@@ -5238,9 +5238,9 @@
       <c r="B22" s="96" t="s">
         <v>93</v>
       </c>
-      <c r="C22" s="95"/>
-      <c r="D22" s="95"/>
-      <c r="E22" s="95"/>
+      <c r="C22" s="92"/>
+      <c r="D22" s="92"/>
+      <c r="E22" s="92"/>
       <c r="F22" s="24"/>
       <c r="K22" s="67"/>
       <c r="L22" s="68"/>
@@ -5249,6 +5249,32 @@
     <row r="23" spans="2:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="I1:O1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
     <mergeCell ref="D22:E22"/>
     <mergeCell ref="D16:E16"/>
     <mergeCell ref="D17:E17"/>
@@ -5265,32 +5291,6 @@
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="I1:O1"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
@@ -5341,18 +5341,18 @@
       </c>
       <c r="D3" s="16">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E3" s="22">
         <f ca="1">SUM(C3:D3)</f>
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="G3" s="23" t="s">
         <v>71</v>
       </c>
       <c r="H3" s="24">
         <f ca="1">VLOOKUP(G3,B2:E31,4,FALSE)</f>
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -5366,11 +5366,11 @@
       </c>
       <c r="D4" s="5">
         <f t="shared" ref="D4:D31" ca="1" si="0">RANDBETWEEN(1,20)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="6">
         <f t="shared" ref="E4:E31" ca="1" si="1">SUM(C4:D4)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
@@ -5384,11 +5384,11 @@
       </c>
       <c r="D5" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E5" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
@@ -5402,11 +5402,11 @@
       </c>
       <c r="D6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E6" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -5420,11 +5420,11 @@
       </c>
       <c r="D7" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -5438,11 +5438,11 @@
       </c>
       <c r="D8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="E8" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -5456,11 +5456,11 @@
       </c>
       <c r="D9" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E9" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
@@ -5492,11 +5492,11 @@
       </c>
       <c r="D11" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E11" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
@@ -5510,11 +5510,11 @@
       </c>
       <c r="D12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
@@ -5528,11 +5528,11 @@
       </c>
       <c r="D13" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="E13" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>7</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
@@ -5546,11 +5546,11 @@
       </c>
       <c r="D14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E14" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
@@ -5564,11 +5564,11 @@
       </c>
       <c r="D15" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E15" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
@@ -5582,11 +5582,11 @@
       </c>
       <c r="D16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E16" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -5600,11 +5600,11 @@
       </c>
       <c r="D17" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
@@ -5618,11 +5618,11 @@
       </c>
       <c r="D18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="E18" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.25">
@@ -5636,11 +5636,11 @@
       </c>
       <c r="D19" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="E19" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.25">
@@ -5672,11 +5672,11 @@
       </c>
       <c r="D21" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E21" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.25">
@@ -5690,11 +5690,11 @@
       </c>
       <c r="D22" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E22" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:5" x14ac:dyDescent="0.25">
@@ -5708,11 +5708,11 @@
       </c>
       <c r="D23" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E23" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="2:5" ht="30" x14ac:dyDescent="0.25">
@@ -5726,11 +5726,11 @@
       </c>
       <c r="D24" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="E24" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="2:5" ht="28.5" x14ac:dyDescent="0.25">
@@ -5744,11 +5744,11 @@
       </c>
       <c r="D25" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E25" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="2:5" ht="45" x14ac:dyDescent="0.25">
@@ -5762,11 +5762,11 @@
       </c>
       <c r="D26" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E26" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="2:5" x14ac:dyDescent="0.25">
@@ -5780,11 +5780,11 @@
       </c>
       <c r="D27" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E27" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="2:5" x14ac:dyDescent="0.25">
@@ -5798,11 +5798,11 @@
       </c>
       <c r="D28" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="E28" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
@@ -5816,11 +5816,11 @@
       </c>
       <c r="D29" s="16">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E29" s="22">
         <f t="shared" ca="1" si="1"/>
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="2:5" x14ac:dyDescent="0.25">
@@ -5834,11 +5834,11 @@
       </c>
       <c r="D30" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E30" s="6">
         <f t="shared" ca="1" si="1"/>
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5852,11 +5852,11 @@
       </c>
       <c r="D31" s="25">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="E31" s="24">
         <f t="shared" ca="1" si="1"/>
-        <v>8</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Após sessão Oferenda 26/04/2025
</commit_message>
<xml_diff>
--- a/Fichas/Tormenta/Ficha Cleber.xlsx
+++ b/Fichas/Tormenta/Ficha Cleber.xlsx
@@ -1618,10 +1618,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;R$&quot;\ * #,##0_-;\-&quot;R$&quot;\ * #,##0_-;_-&quot;R$&quot;\ * &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="28">
     <font>
@@ -1666,9 +1666,121 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1682,63 +1794,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1747,64 +1805,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Aptos Narrow"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Aptos Narrow"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1849,13 +1849,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1873,163 +2023,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2552,50 +2552,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2611,17 +2567,20 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2643,157 +2602,198 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="43" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="45" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="42" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="45" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="44" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="41" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="43" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="38" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="41" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="44" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="40" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="38" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="42" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4398,7 +4398,7 @@
   <dimension ref="B1:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:H10"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -4610,12 +4610,12 @@
       <c r="M8" s="29"/>
       <c r="N8" s="42"/>
     </row>
-    <row r="9" ht="17.25" spans="6:14">
+    <row r="9" spans="6:14">
       <c r="F9" s="38" t="s">
         <v>18</v>
       </c>
       <c r="G9" s="27">
-        <v>320</v>
+        <v>220</v>
       </c>
       <c r="H9" s="39"/>
       <c r="K9" s="38">
@@ -4625,12 +4625,12 @@
       <c r="M9" s="27"/>
       <c r="N9" s="39"/>
     </row>
-    <row r="10" spans="6:14">
+    <row r="10" ht="17.25" spans="6:14">
       <c r="F10" s="45" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="53">
-        <v>6500</v>
+        <v>6600</v>
       </c>
       <c r="H10" s="46"/>
       <c r="K10" s="41">
@@ -5298,18 +5298,18 @@
       </c>
       <c r="D3" s="27">
         <f ca="1">RANDBETWEEN(1,20)</f>
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E3" s="39">
         <f ca="1">SUM(C3:D3)</f>
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="G3" s="43" t="s">
         <v>80</v>
       </c>
       <c r="H3" s="44">
         <f ca="1">VLOOKUP(G3,B2:E31,4,FALSE)</f>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" ht="17.25" spans="2:5">
@@ -5323,11 +5323,11 @@
       </c>
       <c r="D4" s="29">
         <f ca="1" t="shared" ref="D4:D31" si="0">RANDBETWEEN(1,20)</f>
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="42">
         <f ca="1" t="shared" ref="E4:E31" si="1">SUM(C4:D4)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:5">
@@ -5341,11 +5341,11 @@
       </c>
       <c r="D5" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E5" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="2:5">
@@ -5359,11 +5359,11 @@
       </c>
       <c r="D6" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E6" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:5">
@@ -5377,11 +5377,11 @@
       </c>
       <c r="D7" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="2:5">
@@ -5395,11 +5395,11 @@
       </c>
       <c r="D8" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="E8" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:5">
@@ -5413,11 +5413,11 @@
       </c>
       <c r="D9" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="E9" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>28</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -5449,11 +5449,11 @@
       </c>
       <c r="D11" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E11" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -5467,11 +5467,11 @@
       </c>
       <c r="D12" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E12" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:5">
@@ -5485,11 +5485,11 @@
       </c>
       <c r="D13" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="E13" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14" spans="2:5">
@@ -5503,11 +5503,11 @@
       </c>
       <c r="D14" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E14" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="2:5">
@@ -5521,11 +5521,11 @@
       </c>
       <c r="D15" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E15" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="2:5">
@@ -5539,11 +5539,11 @@
       </c>
       <c r="D16" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E16" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:5">
@@ -5557,11 +5557,11 @@
       </c>
       <c r="D17" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E17" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="2:5">
@@ -5575,11 +5575,11 @@
       </c>
       <c r="D18" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E18" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="2:5">
@@ -5593,11 +5593,11 @@
       </c>
       <c r="D19" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E19" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:5">
@@ -5611,11 +5611,11 @@
       </c>
       <c r="D20" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E20" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>20</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="2:5">
@@ -5629,11 +5629,11 @@
       </c>
       <c r="D21" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E21" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="2:5">
@@ -5647,11 +5647,11 @@
       </c>
       <c r="D22" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="E22" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>16</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="2:5">
@@ -5665,11 +5665,11 @@
       </c>
       <c r="D23" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E23" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="2:5">
@@ -5683,11 +5683,11 @@
       </c>
       <c r="D24" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="E24" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="2:5">
@@ -5701,11 +5701,11 @@
       </c>
       <c r="D25" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="E25" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>15</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="2:5">
@@ -5719,11 +5719,11 @@
       </c>
       <c r="D26" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E26" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="2:5">
@@ -5737,11 +5737,11 @@
       </c>
       <c r="D27" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E27" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="2:5">
@@ -5755,11 +5755,11 @@
       </c>
       <c r="D28" s="29">
         <f ca="1" t="shared" si="0"/>
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="E28" s="42">
         <f ca="1" t="shared" si="1"/>
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:5">
@@ -5773,11 +5773,11 @@
       </c>
       <c r="D29" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E29" s="39">
         <f ca="1" t="shared" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:5">
@@ -5809,11 +5809,11 @@
       </c>
       <c r="D31" s="50">
         <f ca="1" t="shared" si="0"/>
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="E31" s="44">
         <f ca="1" t="shared" si="1"/>
-        <v>21</v>
+        <v>12</v>
       </c>
     </row>
     <row r="32" ht="17.25"/>
@@ -5837,7 +5837,7 @@
   <dimension ref="B1:H35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="7"/>
@@ -6302,8 +6302,8 @@
   <sheetPr/>
   <dimension ref="B1:I35"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>
@@ -6763,8 +6763,8 @@
   <sheetPr/>
   <dimension ref="B1:Q33"/>
   <sheetViews>
-    <sheetView zoomScale="88" zoomScaleNormal="88" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView zoomScale="88" zoomScaleNormal="88" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5"/>

</xml_diff>